<commit_message>
added search by rating functionality
</commit_message>
<xml_diff>
--- a/games.xlsx
+++ b/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\PythonProjects\Recommendation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C450148C-E4C7-4EEB-BF93-7316299397CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9D3A99-C064-4A74-A867-302508B894EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D2F7B007-94CF-4E1E-B2CD-4E39721F5B74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -124,9 +124,6 @@
     <t>January 26, 2010</t>
   </si>
   <si>
-    <t>GTA: San Andreas</t>
-  </si>
-  <si>
     <t>October 26, 2004</t>
   </si>
   <si>
@@ -179,6 +176,159 @@
   </si>
   <si>
     <t>PC, Xbox, Android</t>
+  </si>
+  <si>
+    <t>Resident Evil 2</t>
+  </si>
+  <si>
+    <t>January 25, 2019</t>
+  </si>
+  <si>
+    <t>Action, Shooter, Adventure</t>
+  </si>
+  <si>
+    <t>Ori and the Will of the Wisps</t>
+  </si>
+  <si>
+    <t>March 10, 2020</t>
+  </si>
+  <si>
+    <t>PC Xbox, Nintendo</t>
+  </si>
+  <si>
+    <t>The Last of Us Part II</t>
+  </si>
+  <si>
+    <t>June 19, 2020</t>
+  </si>
+  <si>
+    <t>Max Payne</t>
+  </si>
+  <si>
+    <t>July 23, 2001</t>
+  </si>
+  <si>
+    <t>Ghost of Tsushima</t>
+  </si>
+  <si>
+    <t>July 17, 2020</t>
+  </si>
+  <si>
+    <t>Marvel's Spider-Man</t>
+  </si>
+  <si>
+    <t>Metal Gear Solid</t>
+  </si>
+  <si>
+    <t>September 13, 1998</t>
+  </si>
+  <si>
+    <t>Warcraft 3: Reign of Chaos</t>
+  </si>
+  <si>
+    <t>June 1, 2002</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Silent Hill 2</t>
+  </si>
+  <si>
+    <t>September 24, 2001</t>
+  </si>
+  <si>
+    <t>Super Mario Odyssey</t>
+  </si>
+  <si>
+    <t>October 27, 2017</t>
+  </si>
+  <si>
+    <t>Arcade, Platformer</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto: San Andreas (GTA)</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto V (GTA)</t>
+  </si>
+  <si>
+    <t>September 17. 2013</t>
+  </si>
+  <si>
+    <t>Half-Life: Alyx</t>
+  </si>
+  <si>
+    <t>March 23, 2020</t>
+  </si>
+  <si>
+    <t>Elden Ring</t>
+  </si>
+  <si>
+    <t>February 25, 2022</t>
+  </si>
+  <si>
+    <t>Final Fantasy VII (1997)</t>
+  </si>
+  <si>
+    <t>January 31, 1997</t>
+  </si>
+  <si>
+    <t>Diablo II</t>
+  </si>
+  <si>
+    <t>June 29, 2000</t>
+  </si>
+  <si>
+    <t>Need For Speed: Most Wanted</t>
+  </si>
+  <si>
+    <t>Nov 15, 2005</t>
+  </si>
+  <si>
+    <t>Racing, Arcade</t>
+  </si>
+  <si>
+    <t>Metal Gear Solid 3: Snake Eater</t>
+  </si>
+  <si>
+    <t>November 17, 2004</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Playstation, Xbox, Nintendo</t>
+  </si>
+  <si>
+    <t>Heroes of Might and Magic 3: The Restoration of Erathia</t>
+  </si>
+  <si>
+    <t>March 3, 1999</t>
+  </si>
+  <si>
+    <t>Fallout: New Vegas</t>
+  </si>
+  <si>
+    <t>October 19, 2010</t>
+  </si>
+  <si>
+    <t>Action, Shooter, Adventure, RPG</t>
+  </si>
+  <si>
+    <t>October 27, 2002</t>
+  </si>
+  <si>
+    <t>Shadow of the Colossus</t>
+  </si>
+  <si>
+    <t>October 18, 2005</t>
+  </si>
+  <si>
+    <t>Grand Theft Auto: Vice City (GTA)</t>
   </si>
 </sst>
 </file>
@@ -530,17 +680,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987EFDA6-25D6-46B7-8263-8C6EB1BC112A}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -572,10 +722,10 @@
         <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -589,10 +739,10 @@
         <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -606,10 +756,10 @@
         <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -623,10 +773,10 @@
         <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -640,10 +790,10 @@
         <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -657,10 +807,10 @@
         <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -674,10 +824,10 @@
         <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -691,10 +841,10 @@
         <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -708,10 +858,10 @@
         <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -725,10 +875,10 @@
         <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -742,10 +892,10 @@
         <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -759,44 +909,395 @@
         <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
       </c>
       <c r="C14">
         <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
       </c>
       <c r="C15">
         <v>93</v>
       </c>
       <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="E15" t="s">
-        <v>42</v>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19">
+        <v>89</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27">
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28">
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35">
+        <v>94</v>
+      </c>
+      <c r="D35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>